<commit_message>
[taekwon] 몬스터 spell_effect 변경
일반 몬스터 spell_effect 변경
</commit_message>
<xml_diff>
--- a/GameData/Excel/content_map.xlsx
+++ b/GameData/Excel/content_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\문서\GitHub\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0E1070-EE44-4E41-A6E3-DCE27458A368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBFFB62-4BA1-40CE-88B2-D110EE89B413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8652" yWindow="10176" windowWidth="20328" windowHeight="12720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="8655" yWindow="10170" windowWidth="20325" windowHeight="12720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="content_map" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>int</t>
   </si>
@@ -86,10 +86,6 @@
   </si>
   <si>
     <t>battle_boss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20001, 20001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -144,6 +140,30 @@
   <si>
     <t>맵 설명
 - 선택지 표시 용</t>
+  </si>
+  <si>
+    <t>test맵_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test맵_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test맵_엘리트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20001,20001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20002,20003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20003,20101,20003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -235,7 +255,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -258,14 +278,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -285,9 +314,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -325,7 +354,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -431,7 +460,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -573,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -581,25 +610,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.8984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14.69921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="19.3984375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.69921875" style="3"/>
+    <col min="2" max="2" width="19.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="19.375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -609,11 +638,11 @@
       <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>9</v>
@@ -628,16 +657,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -646,172 +675,199 @@
         <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:9" s="8" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="8">
-        <v>20001</v>
+      <c r="D4" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>102</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>103</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13">
+        <v>20003</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>103</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8">
-        <v>20003</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>